<commit_message>
Add Prototype for Buildings & Enemies
</commit_message>
<xml_diff>
--- a/AAAGameData/DataTables/Core/EntityGroupTable.xlsx
+++ b/AAAGameData/DataTables/Core/EntityGroupTable.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B51F33-7F6D-4282-A40B-5FFCB9C3BC86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1323ABC5-ACE6-4702-A17F-74FC4EF55E4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1215" yWindow="2370" windowWidth="16410" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>#</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -115,7 +115,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Billboard</t>
+    <t>Buliding</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enemy</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -470,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -706,6 +710,26 @@
         <v>60</v>
       </c>
       <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13">
+        <v>60</v>
+      </c>
+      <c r="F13">
+        <v>60</v>
+      </c>
+      <c r="G13">
+        <v>60</v>
+      </c>
+      <c r="H13">
         <v>0</v>
       </c>
     </row>

</xml_diff>